<commit_message>
[Update] All APIs are built and tested
</commit_message>
<xml_diff>
--- a/quiz.xlsx
+++ b/quiz.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web_App\Michael\Sapient\Sapient_backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EBE19A-B5D5-46CB-BC35-9E9CB40F94BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18160109-983E-4A30-98A1-084ED10569CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{432E7B59-0DE4-4BC3-9351-DB095DECF0DE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="60">
   <si>
     <t>Question</t>
   </si>
@@ -108,17 +108,110 @@
     <t>Have any of the equipment undergone a sudden increase in power consumption?</t>
   </si>
   <si>
-    <t>What is power consumption of our buildings?</t>
-  </si>
-  <si>
     <t>get_building_energy_consumption_overall</t>
+  </si>
+  <si>
+    <t>get_building_energy_consumption_by_end_uses_category</t>
+  </si>
+  <si>
+    <t>What is the overall energy usage of our building?</t>
+  </si>
+  <si>
+    <t>Can you provide me with the total energy consumed by our building?</t>
+  </si>
+  <si>
+    <t>How much energy does our building consume in total?</t>
+  </si>
+  <si>
+    <t>What is the total energy consumption of our facility?</t>
+  </si>
+  <si>
+    <t>Could you tell me the cumulative energy usage of our entire building?</t>
+  </si>
+  <si>
+    <t>Can you provide the breakdown of the building's energy consumption by end use category?</t>
+  </si>
+  <si>
+    <t>What percentage of the building's energy consumption is attributed to HVAC?</t>
+  </si>
+  <si>
+    <t>How much energy is consumed by lighting in the building?</t>
+  </si>
+  <si>
+    <t>Can you provide the energy usage for process-related activities within the building?</t>
+  </si>
+  <si>
+    <t>What is the energy consumption of plug loads in the building?</t>
+  </si>
+  <si>
+    <t>What is the total energy consumption for lighting in our facility?</t>
+  </si>
+  <si>
+    <t>Can you provide the aggregated energy consumption for our HVAC systems?</t>
+  </si>
+  <si>
+    <t>What is the total energy usage for our production machinery?</t>
+  </si>
+  <si>
+    <t>How much energy is consumed by our office equipment?</t>
+  </si>
+  <si>
+    <t>Can you give me the aggregated energy consumption for cooling?</t>
+  </si>
+  <si>
+    <t>get_energy_building_equipment</t>
+  </si>
+  <si>
+    <t>Return top 5 pieces of equipment that contribute most to whole building energy consumption</t>
+  </si>
+  <si>
+    <t>get_explorer_equip_power_consumption</t>
+  </si>
+  <si>
+    <t>Return top 5 pieces of equipment that contribute most to energy consumption of a specific end use category</t>
+  </si>
+  <si>
+    <t>Return top 5 pieces of equipment that contribute most to energy consumption for a specific equipment type</t>
+  </si>
+  <si>
+    <t>Return top 5 pieces of equipment that contribute most to energy consumption for a specific time period</t>
+  </si>
+  <si>
+    <t>get_hvac_end_use_category_energy_consumption</t>
+  </si>
+  <si>
+    <t>Return [month / week / day / hour] in which energy consumption for HVAC end use category was the highest (and kWh value)</t>
+  </si>
+  <si>
+    <t>get_lighting_end_use_category_energy_consumption</t>
+  </si>
+  <si>
+    <t>get_plug_end_use_category_energy_consumption</t>
+  </si>
+  <si>
+    <t>get_process_end_use_category_energy_consumption</t>
+  </si>
+  <si>
+    <t>get_other_end_use_category_energy_consumption</t>
+  </si>
+  <si>
+    <t>Return [month / week / day / hour] in which energy consumption for Lighting end use category was the highest (and kWh value)</t>
+  </si>
+  <si>
+    <t>Return [month / week / day / hour] in which energy consumption for Plug end use category was the highest (and kWh value)</t>
+  </si>
+  <si>
+    <t>Return [month / week / day / hour] in which energy consumption for Process end use category was the highest (and kWh value)</t>
+  </si>
+  <si>
+    <t>Return [month / week / day / hour] in which energy consumption for Other end use category was the highest (and kWh value)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,8 +225,20 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,13 +247,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -165,11 +300,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -486,17 +645,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{431493E8-EE08-482F-BC87-6266B81F1595}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="121.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="109.5703125" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -510,136 +669,389 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B8" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="B10" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="1" t="s">
+    </row>
+    <row r="14" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Update] Add the question model
</commit_message>
<xml_diff>
--- a/quiz.xlsx
+++ b/quiz.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web_App\Michael\Sapient\Sapient_backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18160109-983E-4A30-98A1-084ED10569CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36524217-2795-4C65-84B2-86C6A77F8688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{432E7B59-0DE4-4BC3-9351-DB095DECF0DE}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{432E7B59-0DE4-4BC3-9351-DB095DECF0DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -288,7 +288,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -296,11 +296,60 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -316,21 +365,32 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -647,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{431493E8-EE08-482F-BC87-6266B81F1595}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,7 +1004,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>43</v>
       </c>
@@ -966,91 +1026,91 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+    <row r="29" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="13" t="s">
+      <c r="B29" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
+    <row r="30" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" s="16" t="s">
+      <c r="B30" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" s="19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
+    <row r="31" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B31" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" s="16" t="s">
+      <c r="B31" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C32" s="19" t="s">
+      <c r="B32" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="22" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C33" s="19" t="s">
+      <c r="B33" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="22" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B34" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C34" s="19" t="s">
+      <c r="B34" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="22" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
+      <c r="A35" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C35" s="19" t="s">
+      <c r="B35" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="22" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
+    <row r="36" spans="1:3" s="26" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36" s="19" t="s">
+      <c r="B36" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="25" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>